<commit_message>
add the option to clear the Constraints file for submit constraints to next week
</commit_message>
<xml_diff>
--- a/workOnExcel/Screwed.xlsx
+++ b/workOnExcel/Screwed.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
   <si>
     <t>index</t>
   </si>
@@ -373,7 +373,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -449,6 +449,22 @@
       </c>
       <c r="B9" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -477,7 +493,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -485,7 +501,7 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -493,7 +509,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -501,7 +517,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -509,7 +525,7 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -517,7 +533,7 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>